<commit_message>
Replace BurnDown_Chart_APPSTACK.xlsx - Meeting 3
</commit_message>
<xml_diff>
--- a/BurnDown_Chart_APPSTACK.xlsx
+++ b/BurnDown_Chart_APPSTACK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annamartin/Desktop/CSE 201/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAE3094-C4DB-4348-AB90-0F4D876F8C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA257B73-D241-0E45-AD31-1B0513FC4561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16320" xr2:uid="{91A116D9-FA0E-DA46-AB0A-A458DF531050}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ideal Track</t>
   </si>
@@ -48,12 +48,36 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Iteration One Tasks</t>
+  </si>
+  <si>
+    <t>Time Estimate</t>
+  </si>
+  <si>
+    <t>Search Bar</t>
+  </si>
+  <si>
+    <t>Scroll Bar</t>
+  </si>
+  <si>
+    <t>Java GUI Window</t>
+  </si>
+  <si>
+    <t>Display Apps</t>
+  </si>
+  <si>
+    <t>Add Details</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,8 +93,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +111,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -133,6 +170,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,10 +385,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,24 +1589,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC00FC1B-D917-0A4A-AE3A-A9992B2A54D3}">
-  <dimension ref="A2:O5"/>
+  <dimension ref="A2:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="16" max="16" width="21.83203125" customWidth="1"/>
+    <col min="17" max="18" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1596,7 +1653,7 @@
       </c>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,22 +1697,38 @@
         <v>0</v>
       </c>
       <c r="O4" s="6"/>
+      <c r="P4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>4</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1663,6 +1736,53 @@
       <c r="M5" s="5"/>
       <c r="N5" s="2"/>
       <c r="O5" s="6"/>
+      <c r="P5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="10">
+        <f>SUM(Q5:Q9)</f>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>